<commit_message>
added data for NL
</commit_message>
<xml_diff>
--- a/data/nl/outcome_table.xlsx
+++ b/data/nl/outcome_table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidpietersz/Documents/GitHub/kansenkloof_NL/data/nl/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lilsonea/Documents/GitHub/Kansenkloof_Nederland/data/nl/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D4E44E03-E95D-CA4D-8E80-62C16FB76CCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D7B4696-D0E0-4D42-BC1D-8BFB304C2E19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{F41B97FE-F77A-4840-B0FB-A5C2C3F09623}"/>
+    <workbookView xWindow="0" yWindow="860" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{F41B97FE-F77A-4840-B0FB-A5C2C3F09623}"/>
   </bookViews>
   <sheets>
     <sheet name="outcome" sheetId="6" r:id="rId1"/>
@@ -28,8 +28,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -37,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1066" uniqueCount="550">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1068" uniqueCount="551">
   <si>
     <t>prefix_postfix</t>
   </si>
@@ -1708,6 +1706,9 @@
   </si>
   <si>
     <t>c11_class_language</t>
+  </si>
+  <si>
+    <t>Nederland</t>
   </si>
 </sst>
 </file>
@@ -1865,9 +1866,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1905,7 +1906,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2011,7 +2012,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2153,7 +2154,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2163,7 +2164,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8F4A81B-7759-BE45-BE6A-975E9F190FD6}">
   <dimension ref="A1:G65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="207" zoomScaleNormal="92" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScaleNormal="92" workbookViewId="0">
       <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
@@ -3480,10 +3481,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08657A33-9ED7-CC48-B84C-CD0BFF48A183}">
-  <dimension ref="A1:B343"/>
+  <dimension ref="A1:B344"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B343"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3502,15 +3503,15 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>207</v>
-      </c>
-      <c r="B2" t="s">
-        <v>519</v>
+        <v>550</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>550</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B3" t="s">
         <v>519</v>
@@ -3518,7 +3519,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B4" t="s">
         <v>519</v>
@@ -3526,7 +3527,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B5" t="s">
         <v>519</v>
@@ -3534,7 +3535,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B6" t="s">
         <v>519</v>
@@ -3542,7 +3543,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B7" t="s">
         <v>519</v>
@@ -3550,7 +3551,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B8" t="s">
         <v>519</v>
@@ -3558,7 +3559,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B9" t="s">
         <v>519</v>
@@ -3566,7 +3567,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B10" t="s">
         <v>519</v>
@@ -3574,7 +3575,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B11" t="s">
         <v>519</v>
@@ -3582,7 +3583,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B12" t="s">
         <v>519</v>
@@ -3590,7 +3591,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B13" t="s">
         <v>519</v>
@@ -3598,15 +3599,15 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>177</v>
+        <v>218</v>
       </c>
       <c r="B14" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>219</v>
+        <v>177</v>
       </c>
       <c r="B15" t="s">
         <v>520</v>
@@ -3614,7 +3615,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>183</v>
+        <v>219</v>
       </c>
       <c r="B16" t="s">
         <v>520</v>
@@ -3622,7 +3623,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>220</v>
+        <v>183</v>
       </c>
       <c r="B17" t="s">
         <v>520</v>
@@ -3630,7 +3631,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B18" t="s">
         <v>520</v>
@@ -3638,7 +3639,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B19" t="s">
         <v>520</v>
@@ -3646,15 +3647,15 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B20" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B21" t="s">
         <v>521</v>
@@ -3662,7 +3663,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B22" t="s">
         <v>521</v>
@@ -3670,7 +3671,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B23" t="s">
         <v>521</v>
@@ -3678,7 +3679,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B24" t="s">
         <v>521</v>
@@ -3686,7 +3687,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B25" t="s">
         <v>521</v>
@@ -3694,7 +3695,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B26" t="s">
         <v>521</v>
@@ -3702,7 +3703,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B27" t="s">
         <v>521</v>
@@ -3710,7 +3711,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B28" t="s">
         <v>521</v>
@@ -3718,7 +3719,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B29" t="s">
         <v>521</v>
@@ -3726,7 +3727,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B30" t="s">
         <v>521</v>
@@ -3734,7 +3735,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B31" t="s">
         <v>521</v>
@@ -3742,7 +3743,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B32" t="s">
         <v>521</v>
@@ -3750,7 +3751,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B33" t="s">
         <v>521</v>
@@ -3758,7 +3759,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B34" t="s">
         <v>521</v>
@@ -3766,7 +3767,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B35" t="s">
         <v>521</v>
@@ -3774,7 +3775,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B36" t="s">
         <v>521</v>
@@ -3782,7 +3783,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B37" t="s">
         <v>521</v>
@@ -3790,15 +3791,15 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B38" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B39" t="s">
         <v>522</v>
@@ -3806,7 +3807,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B40" t="s">
         <v>522</v>
@@ -3814,7 +3815,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B41" t="s">
         <v>522</v>
@@ -3822,7 +3823,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B42" t="s">
         <v>522</v>
@@ -3830,7 +3831,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B43" t="s">
         <v>522</v>
@@ -3838,7 +3839,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B44" t="s">
         <v>522</v>
@@ -3846,7 +3847,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B45" t="s">
         <v>522</v>
@@ -3854,7 +3855,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B46" t="s">
         <v>522</v>
@@ -3862,7 +3863,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B47" t="s">
         <v>522</v>
@@ -3870,7 +3871,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B48" t="s">
         <v>522</v>
@@ -3878,7 +3879,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B49" t="s">
         <v>522</v>
@@ -3886,7 +3887,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B50" t="s">
         <v>522</v>
@@ -3894,7 +3895,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B51" t="s">
         <v>522</v>
@@ -3902,7 +3903,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B52" t="s">
         <v>522</v>
@@ -3910,7 +3911,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B53" t="s">
         <v>522</v>
@@ -3918,7 +3919,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B54" t="s">
         <v>522</v>
@@ -3926,7 +3927,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B55" t="s">
         <v>522</v>
@@ -3934,7 +3935,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B56" t="s">
         <v>522</v>
@@ -3942,7 +3943,7 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B57" t="s">
         <v>522</v>
@@ -3950,7 +3951,7 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B58" t="s">
         <v>522</v>
@@ -3958,7 +3959,7 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B59" t="s">
         <v>522</v>
@@ -3966,7 +3967,7 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B60" t="s">
         <v>522</v>
@@ -3974,7 +3975,7 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B61" t="s">
         <v>522</v>
@@ -3982,7 +3983,7 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B62" t="s">
         <v>522</v>
@@ -3990,7 +3991,7 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B63" t="s">
         <v>522</v>
@@ -3998,7 +3999,7 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B64" t="s">
         <v>522</v>
@@ -4006,7 +4007,7 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B65" t="s">
         <v>522</v>
@@ -4014,7 +4015,7 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B66" t="s">
         <v>522</v>
@@ -4022,7 +4023,7 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B67" t="s">
         <v>522</v>
@@ -4030,7 +4031,7 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B68" t="s">
         <v>522</v>
@@ -4038,7 +4039,7 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B69" t="s">
         <v>522</v>
@@ -4046,7 +4047,7 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B70" t="s">
         <v>522</v>
@@ -4054,7 +4055,7 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B71" t="s">
         <v>522</v>
@@ -4062,7 +4063,7 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B72" t="s">
         <v>522</v>
@@ -4070,7 +4071,7 @@
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B73" t="s">
         <v>522</v>
@@ -4078,7 +4079,7 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B74" t="s">
         <v>522</v>
@@ -4086,7 +4087,7 @@
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B75" t="s">
         <v>522</v>
@@ -4094,7 +4095,7 @@
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B76" t="s">
         <v>522</v>
@@ -4102,7 +4103,7 @@
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B77" t="s">
         <v>522</v>
@@ -4110,7 +4111,7 @@
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B78" t="s">
         <v>522</v>
@@ -4118,7 +4119,7 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B79" t="s">
         <v>522</v>
@@ -4126,7 +4127,7 @@
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B80" t="s">
         <v>522</v>
@@ -4134,7 +4135,7 @@
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B81" t="s">
         <v>522</v>
@@ -4142,7 +4143,7 @@
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B82" t="s">
         <v>522</v>
@@ -4150,7 +4151,7 @@
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B83" t="s">
         <v>522</v>
@@ -4158,7 +4159,7 @@
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B84" t="s">
         <v>522</v>
@@ -4166,7 +4167,7 @@
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B85" t="s">
         <v>522</v>
@@ -4174,7 +4175,7 @@
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B86" t="s">
         <v>522</v>
@@ -4182,7 +4183,7 @@
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B87" t="s">
         <v>522</v>
@@ -4190,7 +4191,7 @@
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B88" t="s">
         <v>522</v>
@@ -4198,15 +4199,15 @@
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B89" t="s">
-        <v>293</v>
+        <v>522</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B90" t="s">
         <v>293</v>
@@ -4214,7 +4215,7 @@
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B91" t="s">
         <v>293</v>
@@ -4222,7 +4223,7 @@
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B92" t="s">
         <v>293</v>
@@ -4230,7 +4231,7 @@
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B93" t="s">
         <v>293</v>
@@ -4238,7 +4239,7 @@
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B94" t="s">
         <v>293</v>
@@ -4246,7 +4247,7 @@
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B95" t="s">
         <v>293</v>
@@ -4254,7 +4255,7 @@
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B96" t="s">
         <v>293</v>
@@ -4262,7 +4263,7 @@
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B97" t="s">
         <v>293</v>
@@ -4270,7 +4271,7 @@
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B98" t="s">
         <v>293</v>
@@ -4278,15 +4279,15 @@
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B99" t="s">
-        <v>523</v>
+        <v>293</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B100" t="s">
         <v>523</v>
@@ -4294,7 +4295,7 @@
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B101" t="s">
         <v>523</v>
@@ -4302,7 +4303,7 @@
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B102" t="s">
         <v>523</v>
@@ -4310,7 +4311,7 @@
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B103" t="s">
         <v>523</v>
@@ -4318,7 +4319,7 @@
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B104" t="s">
         <v>523</v>
@@ -4326,7 +4327,7 @@
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B105" t="s">
         <v>523</v>
@@ -4334,7 +4335,7 @@
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B106" t="s">
         <v>523</v>
@@ -4342,7 +4343,7 @@
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B107" t="s">
         <v>523</v>
@@ -4350,7 +4351,7 @@
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B108" t="s">
         <v>523</v>
@@ -4358,7 +4359,7 @@
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B109" t="s">
         <v>523</v>
@@ -4366,7 +4367,7 @@
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B110" t="s">
         <v>523</v>
@@ -4374,7 +4375,7 @@
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B111" t="s">
         <v>523</v>
@@ -4382,7 +4383,7 @@
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B112" t="s">
         <v>523</v>
@@ -4390,7 +4391,7 @@
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B113" t="s">
         <v>523</v>
@@ -4398,7 +4399,7 @@
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B114" t="s">
         <v>523</v>
@@ -4406,7 +4407,7 @@
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B115" t="s">
         <v>523</v>
@@ -4414,7 +4415,7 @@
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B116" t="s">
         <v>523</v>
@@ -4422,7 +4423,7 @@
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B117" t="s">
         <v>523</v>
@@ -4430,7 +4431,7 @@
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B118" t="s">
         <v>523</v>
@@ -4438,7 +4439,7 @@
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B119" t="s">
         <v>523</v>
@@ -4446,7 +4447,7 @@
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B120" t="s">
         <v>523</v>
@@ -4454,7 +4455,7 @@
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B121" t="s">
         <v>523</v>
@@ -4462,7 +4463,7 @@
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B122" t="s">
         <v>523</v>
@@ -4470,7 +4471,7 @@
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B123" t="s">
         <v>523</v>
@@ -4478,7 +4479,7 @@
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B124" t="s">
         <v>523</v>
@@ -4486,7 +4487,7 @@
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B125" t="s">
         <v>523</v>
@@ -4494,7 +4495,7 @@
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B126" t="s">
         <v>523</v>
@@ -4502,7 +4503,7 @@
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B127" t="s">
         <v>523</v>
@@ -4510,7 +4511,7 @@
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B128" t="s">
         <v>523</v>
@@ -4518,7 +4519,7 @@
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B129" t="s">
         <v>523</v>
@@ -4526,15 +4527,15 @@
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B130" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B131" t="s">
         <v>524</v>
@@ -4542,7 +4543,7 @@
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B132" t="s">
         <v>524</v>
@@ -4550,7 +4551,7 @@
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B133" t="s">
         <v>524</v>
@@ -4558,7 +4559,7 @@
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B134" t="s">
         <v>524</v>
@@ -4566,7 +4567,7 @@
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B135" t="s">
         <v>524</v>
@@ -4574,7 +4575,7 @@
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B136" t="s">
         <v>524</v>
@@ -4582,7 +4583,7 @@
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B137" t="s">
         <v>524</v>
@@ -4590,7 +4591,7 @@
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B138" t="s">
         <v>524</v>
@@ -4598,7 +4599,7 @@
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B139" t="s">
         <v>524</v>
@@ -4606,7 +4607,7 @@
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B140" t="s">
         <v>524</v>
@@ -4614,7 +4615,7 @@
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B141" t="s">
         <v>524</v>
@@ -4622,7 +4623,7 @@
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B142" t="s">
         <v>524</v>
@@ -4630,7 +4631,7 @@
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B143" t="s">
         <v>524</v>
@@ -4638,7 +4639,7 @@
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B144" t="s">
         <v>524</v>
@@ -4646,7 +4647,7 @@
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B145" t="s">
         <v>524</v>
@@ -4654,7 +4655,7 @@
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B146" t="s">
         <v>524</v>
@@ -4662,7 +4663,7 @@
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B147" t="s">
         <v>524</v>
@@ -4670,7 +4671,7 @@
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B148" t="s">
         <v>524</v>
@@ -4678,7 +4679,7 @@
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B149" t="s">
         <v>524</v>
@@ -4686,7 +4687,7 @@
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B150" t="s">
         <v>524</v>
@@ -4694,7 +4695,7 @@
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B151" t="s">
         <v>524</v>
@@ -4702,7 +4703,7 @@
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B152" t="s">
         <v>524</v>
@@ -4710,7 +4711,7 @@
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B153" t="s">
         <v>524</v>
@@ -4718,7 +4719,7 @@
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B154" t="s">
         <v>524</v>
@@ -4726,7 +4727,7 @@
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B155" t="s">
         <v>524</v>
@@ -4734,7 +4735,7 @@
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B156" t="s">
         <v>524</v>
@@ -4742,7 +4743,7 @@
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B157" t="s">
         <v>524</v>
@@ -4750,7 +4751,7 @@
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B158" t="s">
         <v>524</v>
@@ -4758,7 +4759,7 @@
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B159" t="s">
         <v>524</v>
@@ -4766,7 +4767,7 @@
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B160" t="s">
         <v>524</v>
@@ -4774,7 +4775,7 @@
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B161" t="s">
         <v>524</v>
@@ -4782,7 +4783,7 @@
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B162" t="s">
         <v>524</v>
@@ -4790,7 +4791,7 @@
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B163" t="s">
         <v>524</v>
@@ -4798,7 +4799,7 @@
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B164" t="s">
         <v>524</v>
@@ -4806,7 +4807,7 @@
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B165" t="s">
         <v>524</v>
@@ -4814,7 +4815,7 @@
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B166" t="s">
         <v>524</v>
@@ -4822,7 +4823,7 @@
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B167" t="s">
         <v>524</v>
@@ -4830,7 +4831,7 @@
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B168" t="s">
         <v>524</v>
@@ -4838,7 +4839,7 @@
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B169" t="s">
         <v>524</v>
@@ -4846,7 +4847,7 @@
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B170" t="s">
         <v>524</v>
@@ -4854,7 +4855,7 @@
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B171" t="s">
         <v>524</v>
@@ -4862,7 +4863,7 @@
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B172" t="s">
         <v>524</v>
@@ -4870,7 +4871,7 @@
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B173" t="s">
         <v>524</v>
@@ -4878,7 +4879,7 @@
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B174" t="s">
         <v>524</v>
@@ -4886,7 +4887,7 @@
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B175" t="s">
         <v>524</v>
@@ -4894,7 +4895,7 @@
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B176" t="s">
         <v>524</v>
@@ -4902,7 +4903,7 @@
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B177" t="s">
         <v>524</v>
@@ -4910,7 +4911,7 @@
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B178" t="s">
         <v>524</v>
@@ -4918,7 +4919,7 @@
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B179" t="s">
         <v>524</v>
@@ -4926,7 +4927,7 @@
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B180" t="s">
         <v>524</v>
@@ -4934,7 +4935,7 @@
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B181" t="s">
         <v>524</v>
@@ -4942,7 +4943,7 @@
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B182" t="s">
         <v>524</v>
@@ -4950,7 +4951,7 @@
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B183" t="s">
         <v>524</v>
@@ -4958,7 +4959,7 @@
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B184" t="s">
         <v>524</v>
@@ -4966,7 +4967,7 @@
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B185" t="s">
         <v>524</v>
@@ -4974,15 +4975,15 @@
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>188</v>
+        <v>388</v>
       </c>
       <c r="B186" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>389</v>
+        <v>188</v>
       </c>
       <c r="B187" t="s">
         <v>525</v>
@@ -4990,7 +4991,7 @@
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>178</v>
+        <v>389</v>
       </c>
       <c r="B188" t="s">
         <v>525</v>
@@ -4998,7 +4999,7 @@
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B189" t="s">
         <v>525</v>
@@ -5006,7 +5007,7 @@
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>390</v>
+        <v>176</v>
       </c>
       <c r="B190" t="s">
         <v>525</v>
@@ -5014,7 +5015,7 @@
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>179</v>
+        <v>390</v>
       </c>
       <c r="B191" t="s">
         <v>525</v>
@@ -5022,7 +5023,7 @@
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>204</v>
+        <v>179</v>
       </c>
       <c r="B192" t="s">
         <v>525</v>
@@ -5030,7 +5031,7 @@
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>193</v>
+        <v>204</v>
       </c>
       <c r="B193" t="s">
         <v>525</v>
@@ -5038,7 +5039,7 @@
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>391</v>
+        <v>193</v>
       </c>
       <c r="B194" t="s">
         <v>525</v>
@@ -5046,7 +5047,7 @@
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>197</v>
+        <v>391</v>
       </c>
       <c r="B195" t="s">
         <v>525</v>
@@ -5054,7 +5055,7 @@
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>392</v>
+        <v>197</v>
       </c>
       <c r="B196" t="s">
         <v>525</v>
@@ -5062,7 +5063,7 @@
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B197" t="s">
         <v>525</v>
@@ -5070,7 +5071,7 @@
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>187</v>
+        <v>393</v>
       </c>
       <c r="B198" t="s">
         <v>525</v>
@@ -5078,7 +5079,7 @@
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>394</v>
+        <v>187</v>
       </c>
       <c r="B199" t="s">
         <v>525</v>
@@ -5086,7 +5087,7 @@
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>180</v>
+        <v>394</v>
       </c>
       <c r="B200" t="s">
         <v>525</v>
@@ -5094,7 +5095,7 @@
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B201" t="s">
         <v>525</v>
@@ -5102,7 +5103,7 @@
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B202" t="s">
         <v>525</v>
@@ -5110,7 +5111,7 @@
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="B203" t="s">
         <v>525</v>
@@ -5118,7 +5119,7 @@
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="B204" t="s">
         <v>525</v>
@@ -5126,7 +5127,7 @@
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
-        <v>395</v>
+        <v>194</v>
       </c>
       <c r="B205" t="s">
         <v>525</v>
@@ -5134,7 +5135,7 @@
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B206" t="s">
         <v>525</v>
@@ -5142,7 +5143,7 @@
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
-        <v>190</v>
+        <v>396</v>
       </c>
       <c r="B207" t="s">
         <v>525</v>
@@ -5150,7 +5151,7 @@
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
-        <v>397</v>
+        <v>190</v>
       </c>
       <c r="B208" t="s">
         <v>525</v>
@@ -5158,7 +5159,7 @@
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B209" t="s">
         <v>525</v>
@@ -5166,7 +5167,7 @@
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
-        <v>191</v>
+        <v>398</v>
       </c>
       <c r="B210" t="s">
         <v>525</v>
@@ -5174,7 +5175,7 @@
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
-        <v>399</v>
+        <v>191</v>
       </c>
       <c r="B211" t="s">
         <v>525</v>
@@ -5182,7 +5183,7 @@
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
-        <v>202</v>
+        <v>399</v>
       </c>
       <c r="B212" t="s">
         <v>525</v>
@@ -5190,7 +5191,7 @@
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B213" t="s">
         <v>525</v>
@@ -5198,7 +5199,7 @@
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
-        <v>400</v>
+        <v>205</v>
       </c>
       <c r="B214" t="s">
         <v>525</v>
@@ -5206,7 +5207,7 @@
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
-        <v>203</v>
+        <v>400</v>
       </c>
       <c r="B215" t="s">
         <v>525</v>
@@ -5214,7 +5215,7 @@
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
-        <v>401</v>
+        <v>203</v>
       </c>
       <c r="B216" t="s">
         <v>525</v>
@@ -5222,7 +5223,7 @@
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
-        <v>201</v>
+        <v>401</v>
       </c>
       <c r="B217" t="s">
         <v>525</v>
@@ -5230,7 +5231,7 @@
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
-        <v>184</v>
+        <v>201</v>
       </c>
       <c r="B218" t="s">
         <v>525</v>
@@ -5238,7 +5239,7 @@
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
-        <v>402</v>
+        <v>184</v>
       </c>
       <c r="B219" t="s">
         <v>525</v>
@@ -5246,7 +5247,7 @@
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B220" t="s">
         <v>525</v>
@@ -5254,7 +5255,7 @@
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B221" t="s">
         <v>525</v>
@@ -5262,7 +5263,7 @@
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
-        <v>199</v>
+        <v>404</v>
       </c>
       <c r="B222" t="s">
         <v>525</v>
@@ -5270,7 +5271,7 @@
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
-        <v>192</v>
+        <v>199</v>
       </c>
       <c r="B223" t="s">
         <v>525</v>
@@ -5278,7 +5279,7 @@
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
-        <v>185</v>
+        <v>192</v>
       </c>
       <c r="B224" t="s">
         <v>525</v>
@@ -5286,7 +5287,7 @@
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
-        <v>198</v>
+        <v>185</v>
       </c>
       <c r="B225" t="s">
         <v>525</v>
@@ -5294,7 +5295,7 @@
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="B226" t="s">
         <v>525</v>
@@ -5302,7 +5303,7 @@
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B227" t="s">
         <v>525</v>
@@ -5310,7 +5311,7 @@
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
-        <v>186</v>
+        <v>196</v>
       </c>
       <c r="B228" t="s">
         <v>525</v>
@@ -5318,7 +5319,7 @@
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
-        <v>200</v>
+        <v>186</v>
       </c>
       <c r="B229" t="s">
         <v>525</v>
@@ -5326,15 +5327,15 @@
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
-        <v>405</v>
+        <v>200</v>
       </c>
       <c r="B230" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B231" t="s">
         <v>526</v>
@@ -5342,7 +5343,7 @@
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B232" t="s">
         <v>526</v>
@@ -5350,7 +5351,7 @@
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B233" t="s">
         <v>526</v>
@@ -5358,7 +5359,7 @@
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B234" t="s">
         <v>526</v>
@@ -5366,7 +5367,7 @@
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B235" t="s">
         <v>526</v>
@@ -5374,7 +5375,7 @@
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B236" t="s">
         <v>526</v>
@@ -5382,7 +5383,7 @@
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B237" t="s">
         <v>526</v>
@@ -5390,7 +5391,7 @@
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B238" t="s">
         <v>526</v>
@@ -5398,7 +5399,7 @@
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B239" t="s">
         <v>526</v>
@@ -5406,7 +5407,7 @@
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B240" t="s">
         <v>526</v>
@@ -5414,7 +5415,7 @@
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B241" t="s">
         <v>526</v>
@@ -5422,7 +5423,7 @@
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B242" t="s">
         <v>526</v>
@@ -5430,7 +5431,7 @@
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B243" t="s">
         <v>526</v>
@@ -5438,7 +5439,7 @@
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B244" t="s">
         <v>526</v>
@@ -5446,7 +5447,7 @@
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B245" t="s">
         <v>526</v>
@@ -5454,7 +5455,7 @@
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B246" t="s">
         <v>526</v>
@@ -5462,7 +5463,7 @@
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B247" t="s">
         <v>526</v>
@@ -5470,7 +5471,7 @@
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B248" t="s">
         <v>526</v>
@@ -5478,7 +5479,7 @@
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B249" t="s">
         <v>526</v>
@@ -5486,7 +5487,7 @@
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B250" t="s">
         <v>526</v>
@@ -5494,7 +5495,7 @@
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B251" t="s">
         <v>526</v>
@@ -5502,7 +5503,7 @@
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B252" t="s">
         <v>526</v>
@@ -5510,7 +5511,7 @@
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B253" t="s">
         <v>526</v>
@@ -5518,7 +5519,7 @@
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B254" t="s">
         <v>526</v>
@@ -5526,15 +5527,15 @@
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B255" t="s">
-        <v>448</v>
+        <v>526</v>
       </c>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B256" t="s">
         <v>448</v>
@@ -5542,7 +5543,7 @@
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B257" t="s">
         <v>448</v>
@@ -5550,7 +5551,7 @@
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B258" t="s">
         <v>448</v>
@@ -5558,7 +5559,7 @@
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B259" t="s">
         <v>448</v>
@@ -5566,7 +5567,7 @@
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B260" t="s">
         <v>448</v>
@@ -5574,7 +5575,7 @@
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B261" t="s">
         <v>448</v>
@@ -5582,7 +5583,7 @@
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B262" t="s">
         <v>448</v>
@@ -5590,7 +5591,7 @@
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B263" t="s">
         <v>448</v>
@@ -5598,7 +5599,7 @@
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A264" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B264" t="s">
         <v>448</v>
@@ -5606,7 +5607,7 @@
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B265" t="s">
         <v>448</v>
@@ -5614,7 +5615,7 @@
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A266" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B266" t="s">
         <v>448</v>
@@ -5622,7 +5623,7 @@
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A267" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B267" t="s">
         <v>448</v>
@@ -5630,7 +5631,7 @@
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A268" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B268" t="s">
         <v>448</v>
@@ -5638,7 +5639,7 @@
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A269" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B269" t="s">
         <v>448</v>
@@ -5646,7 +5647,7 @@
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A270" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B270" t="s">
         <v>448</v>
@@ -5654,7 +5655,7 @@
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A271" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B271" t="s">
         <v>448</v>
@@ -5662,7 +5663,7 @@
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A272" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B272" t="s">
         <v>448</v>
@@ -5670,7 +5671,7 @@
     </row>
     <row r="273" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A273" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B273" t="s">
         <v>448</v>
@@ -5678,7 +5679,7 @@
     </row>
     <row r="274" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A274" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B274" t="s">
         <v>448</v>
@@ -5686,7 +5687,7 @@
     </row>
     <row r="275" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A275" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B275" t="s">
         <v>448</v>
@@ -5694,7 +5695,7 @@
     </row>
     <row r="276" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A276" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B276" t="s">
         <v>448</v>
@@ -5702,7 +5703,7 @@
     </row>
     <row r="277" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A277" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B277" t="s">
         <v>448</v>
@@ -5710,7 +5711,7 @@
     </row>
     <row r="278" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A278" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B278" t="s">
         <v>448</v>
@@ -5718,7 +5719,7 @@
     </row>
     <row r="279" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A279" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B279" t="s">
         <v>448</v>
@@ -5726,7 +5727,7 @@
     </row>
     <row r="280" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A280" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B280" t="s">
         <v>448</v>
@@ -5734,15 +5735,15 @@
     </row>
     <row r="281" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A281" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B281" t="s">
-        <v>527</v>
+        <v>448</v>
       </c>
     </row>
     <row r="282" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A282" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B282" t="s">
         <v>527</v>
@@ -5750,7 +5751,7 @@
     </row>
     <row r="283" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A283" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B283" t="s">
         <v>527</v>
@@ -5758,7 +5759,7 @@
     </row>
     <row r="284" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A284" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B284" t="s">
         <v>527</v>
@@ -5766,7 +5767,7 @@
     </row>
     <row r="285" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A285" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B285" t="s">
         <v>527</v>
@@ -5774,7 +5775,7 @@
     </row>
     <row r="286" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A286" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B286" t="s">
         <v>527</v>
@@ -5782,7 +5783,7 @@
     </row>
     <row r="287" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A287" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B287" t="s">
         <v>527</v>
@@ -5790,7 +5791,7 @@
     </row>
     <row r="288" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A288" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B288" t="s">
         <v>527</v>
@@ -5798,7 +5799,7 @@
     </row>
     <row r="289" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A289" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B289" t="s">
         <v>527</v>
@@ -5806,7 +5807,7 @@
     </row>
     <row r="290" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A290" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B290" t="s">
         <v>527</v>
@@ -5814,7 +5815,7 @@
     </row>
     <row r="291" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A291" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B291" t="s">
         <v>527</v>
@@ -5822,7 +5823,7 @@
     </row>
     <row r="292" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A292" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B292" t="s">
         <v>527</v>
@@ -5830,7 +5831,7 @@
     </row>
     <row r="293" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A293" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B293" t="s">
         <v>527</v>
@@ -5838,15 +5839,15 @@
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A294" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B294" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="295" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A295" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B295" t="s">
         <v>528</v>
@@ -5854,7 +5855,7 @@
     </row>
     <row r="296" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A296" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B296" t="s">
         <v>528</v>
@@ -5862,7 +5863,7 @@
     </row>
     <row r="297" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A297" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B297" t="s">
         <v>528</v>
@@ -5870,7 +5871,7 @@
     </row>
     <row r="298" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A298" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B298" t="s">
         <v>528</v>
@@ -5878,7 +5879,7 @@
     </row>
     <row r="299" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A299" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B299" t="s">
         <v>528</v>
@@ -5886,7 +5887,7 @@
     </row>
     <row r="300" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A300" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B300" t="s">
         <v>528</v>
@@ -5894,7 +5895,7 @@
     </row>
     <row r="301" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A301" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B301" t="s">
         <v>528</v>
@@ -5902,7 +5903,7 @@
     </row>
     <row r="302" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A302" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B302" t="s">
         <v>528</v>
@@ -5910,7 +5911,7 @@
     </row>
     <row r="303" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A303" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B303" t="s">
         <v>528</v>
@@ -5918,7 +5919,7 @@
     </row>
     <row r="304" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A304" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B304" t="s">
         <v>528</v>
@@ -5926,7 +5927,7 @@
     </row>
     <row r="305" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A305" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B305" t="s">
         <v>528</v>
@@ -5934,7 +5935,7 @@
     </row>
     <row r="306" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A306" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B306" t="s">
         <v>528</v>
@@ -5942,7 +5943,7 @@
     </row>
     <row r="307" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A307" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B307" t="s">
         <v>528</v>
@@ -5950,7 +5951,7 @@
     </row>
     <row r="308" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A308" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B308" t="s">
         <v>528</v>
@@ -5958,7 +5959,7 @@
     </row>
     <row r="309" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A309" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B309" t="s">
         <v>528</v>
@@ -5966,7 +5967,7 @@
     </row>
     <row r="310" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A310" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="B310" t="s">
         <v>528</v>
@@ -5974,7 +5975,7 @@
     </row>
     <row r="311" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A311" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B311" t="s">
         <v>528</v>
@@ -5982,7 +5983,7 @@
     </row>
     <row r="312" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A312" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B312" t="s">
         <v>528</v>
@@ -5990,7 +5991,7 @@
     </row>
     <row r="313" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A313" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B313" t="s">
         <v>528</v>
@@ -5998,7 +5999,7 @@
     </row>
     <row r="314" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A314" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B314" t="s">
         <v>528</v>
@@ -6006,7 +6007,7 @@
     </row>
     <row r="315" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A315" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B315" t="s">
         <v>528</v>
@@ -6014,7 +6015,7 @@
     </row>
     <row r="316" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A316" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B316" t="s">
         <v>528</v>
@@ -6022,7 +6023,7 @@
     </row>
     <row r="317" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A317" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B317" t="s">
         <v>528</v>
@@ -6030,7 +6031,7 @@
     </row>
     <row r="318" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A318" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="B318" t="s">
         <v>528</v>
@@ -6038,7 +6039,7 @@
     </row>
     <row r="319" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A319" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B319" t="s">
         <v>528</v>
@@ -6046,7 +6047,7 @@
     </row>
     <row r="320" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A320" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B320" t="s">
         <v>528</v>
@@ -6054,7 +6055,7 @@
     </row>
     <row r="321" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A321" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B321" t="s">
         <v>528</v>
@@ -6062,7 +6063,7 @@
     </row>
     <row r="322" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A322" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B322" t="s">
         <v>528</v>
@@ -6070,7 +6071,7 @@
     </row>
     <row r="323" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A323" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B323" t="s">
         <v>528</v>
@@ -6078,7 +6079,7 @@
     </row>
     <row r="324" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A324" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="B324" t="s">
         <v>528</v>
@@ -6086,7 +6087,7 @@
     </row>
     <row r="325" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A325" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="B325" t="s">
         <v>528</v>
@@ -6094,7 +6095,7 @@
     </row>
     <row r="326" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A326" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="B326" t="s">
         <v>528</v>
@@ -6102,7 +6103,7 @@
     </row>
     <row r="327" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A327" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="B327" t="s">
         <v>528</v>
@@ -6110,7 +6111,7 @@
     </row>
     <row r="328" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A328" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="B328" t="s">
         <v>528</v>
@@ -6118,7 +6119,7 @@
     </row>
     <row r="329" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A329" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="B329" t="s">
         <v>528</v>
@@ -6126,7 +6127,7 @@
     </row>
     <row r="330" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A330" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="B330" t="s">
         <v>528</v>
@@ -6134,7 +6135,7 @@
     </row>
     <row r="331" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A331" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="B331" t="s">
         <v>528</v>
@@ -6142,7 +6143,7 @@
     </row>
     <row r="332" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A332" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="B332" t="s">
         <v>528</v>
@@ -6150,7 +6151,7 @@
     </row>
     <row r="333" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A333" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="B333" t="s">
         <v>528</v>
@@ -6158,7 +6159,7 @@
     </row>
     <row r="334" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A334" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B334" t="s">
         <v>528</v>
@@ -6166,7 +6167,7 @@
     </row>
     <row r="335" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A335" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B335" t="s">
         <v>528</v>
@@ -6174,7 +6175,7 @@
     </row>
     <row r="336" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A336" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="B336" t="s">
         <v>528</v>
@@ -6182,7 +6183,7 @@
     </row>
     <row r="337" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A337" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B337" t="s">
         <v>528</v>
@@ -6190,7 +6191,7 @@
     </row>
     <row r="338" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A338" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="B338" t="s">
         <v>528</v>
@@ -6198,7 +6199,7 @@
     </row>
     <row r="339" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A339" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="B339" t="s">
         <v>528</v>
@@ -6206,7 +6207,7 @@
     </row>
     <row r="340" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A340" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B340" t="s">
         <v>528</v>
@@ -6214,7 +6215,7 @@
     </row>
     <row r="341" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A341" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B341" t="s">
         <v>528</v>
@@ -6222,7 +6223,7 @@
     </row>
     <row r="342" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A342" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B342" t="s">
         <v>528</v>
@@ -6230,9 +6231,17 @@
     </row>
     <row r="343" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A343" t="s">
+        <v>517</v>
+      </c>
+      <c r="B343" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="344" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A344" t="s">
         <v>518</v>
       </c>
-      <c r="B343" t="s">
+      <c r="B344" t="s">
         <v>528</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed interface to show Friesland, added the whole of the Netherlands
</commit_message>
<xml_diff>
--- a/data/nl/outcome_table.xlsx
+++ b/data/nl/outcome_table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidpietersz/Documents/GitHub/kansenkloof_NL/data/nl/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lilsonea/Documents/GitHub/Kansenkloof_Nederland/data/nl/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D4E44E03-E95D-CA4D-8E80-62C16FB76CCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D7B4696-D0E0-4D42-BC1D-8BFB304C2E19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{F41B97FE-F77A-4840-B0FB-A5C2C3F09623}"/>
+    <workbookView xWindow="0" yWindow="860" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{F41B97FE-F77A-4840-B0FB-A5C2C3F09623}"/>
   </bookViews>
   <sheets>
     <sheet name="outcome" sheetId="6" r:id="rId1"/>
@@ -28,8 +28,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -37,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1066" uniqueCount="550">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1068" uniqueCount="551">
   <si>
     <t>prefix_postfix</t>
   </si>
@@ -1708,6 +1706,9 @@
   </si>
   <si>
     <t>c11_class_language</t>
+  </si>
+  <si>
+    <t>Nederland</t>
   </si>
 </sst>
 </file>
@@ -1865,9 +1866,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1905,7 +1906,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2011,7 +2012,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2153,7 +2154,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2163,7 +2164,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8F4A81B-7759-BE45-BE6A-975E9F190FD6}">
   <dimension ref="A1:G65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="207" zoomScaleNormal="92" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScaleNormal="92" workbookViewId="0">
       <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
@@ -3480,10 +3481,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08657A33-9ED7-CC48-B84C-CD0BFF48A183}">
-  <dimension ref="A1:B343"/>
+  <dimension ref="A1:B344"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B343"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3502,15 +3503,15 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>207</v>
-      </c>
-      <c r="B2" t="s">
-        <v>519</v>
+        <v>550</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>550</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B3" t="s">
         <v>519</v>
@@ -3518,7 +3519,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B4" t="s">
         <v>519</v>
@@ -3526,7 +3527,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B5" t="s">
         <v>519</v>
@@ -3534,7 +3535,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B6" t="s">
         <v>519</v>
@@ -3542,7 +3543,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B7" t="s">
         <v>519</v>
@@ -3550,7 +3551,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B8" t="s">
         <v>519</v>
@@ -3558,7 +3559,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B9" t="s">
         <v>519</v>
@@ -3566,7 +3567,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B10" t="s">
         <v>519</v>
@@ -3574,7 +3575,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B11" t="s">
         <v>519</v>
@@ -3582,7 +3583,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B12" t="s">
         <v>519</v>
@@ -3590,7 +3591,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B13" t="s">
         <v>519</v>
@@ -3598,15 +3599,15 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>177</v>
+        <v>218</v>
       </c>
       <c r="B14" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>219</v>
+        <v>177</v>
       </c>
       <c r="B15" t="s">
         <v>520</v>
@@ -3614,7 +3615,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>183</v>
+        <v>219</v>
       </c>
       <c r="B16" t="s">
         <v>520</v>
@@ -3622,7 +3623,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>220</v>
+        <v>183</v>
       </c>
       <c r="B17" t="s">
         <v>520</v>
@@ -3630,7 +3631,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B18" t="s">
         <v>520</v>
@@ -3638,7 +3639,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B19" t="s">
         <v>520</v>
@@ -3646,15 +3647,15 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B20" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B21" t="s">
         <v>521</v>
@@ -3662,7 +3663,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B22" t="s">
         <v>521</v>
@@ -3670,7 +3671,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B23" t="s">
         <v>521</v>
@@ -3678,7 +3679,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B24" t="s">
         <v>521</v>
@@ -3686,7 +3687,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B25" t="s">
         <v>521</v>
@@ -3694,7 +3695,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B26" t="s">
         <v>521</v>
@@ -3702,7 +3703,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B27" t="s">
         <v>521</v>
@@ -3710,7 +3711,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B28" t="s">
         <v>521</v>
@@ -3718,7 +3719,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B29" t="s">
         <v>521</v>
@@ -3726,7 +3727,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B30" t="s">
         <v>521</v>
@@ -3734,7 +3735,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B31" t="s">
         <v>521</v>
@@ -3742,7 +3743,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B32" t="s">
         <v>521</v>
@@ -3750,7 +3751,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B33" t="s">
         <v>521</v>
@@ -3758,7 +3759,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B34" t="s">
         <v>521</v>
@@ -3766,7 +3767,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B35" t="s">
         <v>521</v>
@@ -3774,7 +3775,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B36" t="s">
         <v>521</v>
@@ -3782,7 +3783,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B37" t="s">
         <v>521</v>
@@ -3790,15 +3791,15 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B38" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B39" t="s">
         <v>522</v>
@@ -3806,7 +3807,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B40" t="s">
         <v>522</v>
@@ -3814,7 +3815,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B41" t="s">
         <v>522</v>
@@ -3822,7 +3823,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B42" t="s">
         <v>522</v>
@@ -3830,7 +3831,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B43" t="s">
         <v>522</v>
@@ -3838,7 +3839,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B44" t="s">
         <v>522</v>
@@ -3846,7 +3847,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B45" t="s">
         <v>522</v>
@@ -3854,7 +3855,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B46" t="s">
         <v>522</v>
@@ -3862,7 +3863,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B47" t="s">
         <v>522</v>
@@ -3870,7 +3871,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B48" t="s">
         <v>522</v>
@@ -3878,7 +3879,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B49" t="s">
         <v>522</v>
@@ -3886,7 +3887,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B50" t="s">
         <v>522</v>
@@ -3894,7 +3895,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B51" t="s">
         <v>522</v>
@@ -3902,7 +3903,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B52" t="s">
         <v>522</v>
@@ -3910,7 +3911,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B53" t="s">
         <v>522</v>
@@ -3918,7 +3919,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B54" t="s">
         <v>522</v>
@@ -3926,7 +3927,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B55" t="s">
         <v>522</v>
@@ -3934,7 +3935,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B56" t="s">
         <v>522</v>
@@ -3942,7 +3943,7 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B57" t="s">
         <v>522</v>
@@ -3950,7 +3951,7 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B58" t="s">
         <v>522</v>
@@ -3958,7 +3959,7 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B59" t="s">
         <v>522</v>
@@ -3966,7 +3967,7 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B60" t="s">
         <v>522</v>
@@ -3974,7 +3975,7 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B61" t="s">
         <v>522</v>
@@ -3982,7 +3983,7 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B62" t="s">
         <v>522</v>
@@ -3990,7 +3991,7 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B63" t="s">
         <v>522</v>
@@ -3998,7 +3999,7 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B64" t="s">
         <v>522</v>
@@ -4006,7 +4007,7 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B65" t="s">
         <v>522</v>
@@ -4014,7 +4015,7 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B66" t="s">
         <v>522</v>
@@ -4022,7 +4023,7 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B67" t="s">
         <v>522</v>
@@ -4030,7 +4031,7 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B68" t="s">
         <v>522</v>
@@ -4038,7 +4039,7 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B69" t="s">
         <v>522</v>
@@ -4046,7 +4047,7 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B70" t="s">
         <v>522</v>
@@ -4054,7 +4055,7 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B71" t="s">
         <v>522</v>
@@ -4062,7 +4063,7 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B72" t="s">
         <v>522</v>
@@ -4070,7 +4071,7 @@
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B73" t="s">
         <v>522</v>
@@ -4078,7 +4079,7 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B74" t="s">
         <v>522</v>
@@ -4086,7 +4087,7 @@
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B75" t="s">
         <v>522</v>
@@ -4094,7 +4095,7 @@
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B76" t="s">
         <v>522</v>
@@ -4102,7 +4103,7 @@
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B77" t="s">
         <v>522</v>
@@ -4110,7 +4111,7 @@
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B78" t="s">
         <v>522</v>
@@ -4118,7 +4119,7 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B79" t="s">
         <v>522</v>
@@ -4126,7 +4127,7 @@
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B80" t="s">
         <v>522</v>
@@ -4134,7 +4135,7 @@
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B81" t="s">
         <v>522</v>
@@ -4142,7 +4143,7 @@
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B82" t="s">
         <v>522</v>
@@ -4150,7 +4151,7 @@
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B83" t="s">
         <v>522</v>
@@ -4158,7 +4159,7 @@
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B84" t="s">
         <v>522</v>
@@ -4166,7 +4167,7 @@
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B85" t="s">
         <v>522</v>
@@ -4174,7 +4175,7 @@
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B86" t="s">
         <v>522</v>
@@ -4182,7 +4183,7 @@
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B87" t="s">
         <v>522</v>
@@ -4190,7 +4191,7 @@
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B88" t="s">
         <v>522</v>
@@ -4198,15 +4199,15 @@
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B89" t="s">
-        <v>293</v>
+        <v>522</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B90" t="s">
         <v>293</v>
@@ -4214,7 +4215,7 @@
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B91" t="s">
         <v>293</v>
@@ -4222,7 +4223,7 @@
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B92" t="s">
         <v>293</v>
@@ -4230,7 +4231,7 @@
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B93" t="s">
         <v>293</v>
@@ -4238,7 +4239,7 @@
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B94" t="s">
         <v>293</v>
@@ -4246,7 +4247,7 @@
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B95" t="s">
         <v>293</v>
@@ -4254,7 +4255,7 @@
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B96" t="s">
         <v>293</v>
@@ -4262,7 +4263,7 @@
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B97" t="s">
         <v>293</v>
@@ -4270,7 +4271,7 @@
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B98" t="s">
         <v>293</v>
@@ -4278,15 +4279,15 @@
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B99" t="s">
-        <v>523</v>
+        <v>293</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B100" t="s">
         <v>523</v>
@@ -4294,7 +4295,7 @@
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B101" t="s">
         <v>523</v>
@@ -4302,7 +4303,7 @@
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B102" t="s">
         <v>523</v>
@@ -4310,7 +4311,7 @@
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B103" t="s">
         <v>523</v>
@@ -4318,7 +4319,7 @@
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B104" t="s">
         <v>523</v>
@@ -4326,7 +4327,7 @@
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B105" t="s">
         <v>523</v>
@@ -4334,7 +4335,7 @@
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B106" t="s">
         <v>523</v>
@@ -4342,7 +4343,7 @@
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B107" t="s">
         <v>523</v>
@@ -4350,7 +4351,7 @@
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B108" t="s">
         <v>523</v>
@@ -4358,7 +4359,7 @@
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B109" t="s">
         <v>523</v>
@@ -4366,7 +4367,7 @@
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B110" t="s">
         <v>523</v>
@@ -4374,7 +4375,7 @@
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B111" t="s">
         <v>523</v>
@@ -4382,7 +4383,7 @@
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B112" t="s">
         <v>523</v>
@@ -4390,7 +4391,7 @@
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B113" t="s">
         <v>523</v>
@@ -4398,7 +4399,7 @@
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B114" t="s">
         <v>523</v>
@@ -4406,7 +4407,7 @@
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B115" t="s">
         <v>523</v>
@@ -4414,7 +4415,7 @@
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B116" t="s">
         <v>523</v>
@@ -4422,7 +4423,7 @@
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B117" t="s">
         <v>523</v>
@@ -4430,7 +4431,7 @@
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B118" t="s">
         <v>523</v>
@@ -4438,7 +4439,7 @@
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B119" t="s">
         <v>523</v>
@@ -4446,7 +4447,7 @@
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B120" t="s">
         <v>523</v>
@@ -4454,7 +4455,7 @@
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B121" t="s">
         <v>523</v>
@@ -4462,7 +4463,7 @@
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B122" t="s">
         <v>523</v>
@@ -4470,7 +4471,7 @@
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B123" t="s">
         <v>523</v>
@@ -4478,7 +4479,7 @@
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B124" t="s">
         <v>523</v>
@@ -4486,7 +4487,7 @@
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B125" t="s">
         <v>523</v>
@@ -4494,7 +4495,7 @@
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B126" t="s">
         <v>523</v>
@@ -4502,7 +4503,7 @@
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B127" t="s">
         <v>523</v>
@@ -4510,7 +4511,7 @@
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B128" t="s">
         <v>523</v>
@@ -4518,7 +4519,7 @@
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B129" t="s">
         <v>523</v>
@@ -4526,15 +4527,15 @@
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B130" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B131" t="s">
         <v>524</v>
@@ -4542,7 +4543,7 @@
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B132" t="s">
         <v>524</v>
@@ -4550,7 +4551,7 @@
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B133" t="s">
         <v>524</v>
@@ -4558,7 +4559,7 @@
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B134" t="s">
         <v>524</v>
@@ -4566,7 +4567,7 @@
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B135" t="s">
         <v>524</v>
@@ -4574,7 +4575,7 @@
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B136" t="s">
         <v>524</v>
@@ -4582,7 +4583,7 @@
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B137" t="s">
         <v>524</v>
@@ -4590,7 +4591,7 @@
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B138" t="s">
         <v>524</v>
@@ -4598,7 +4599,7 @@
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B139" t="s">
         <v>524</v>
@@ -4606,7 +4607,7 @@
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B140" t="s">
         <v>524</v>
@@ -4614,7 +4615,7 @@
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B141" t="s">
         <v>524</v>
@@ -4622,7 +4623,7 @@
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B142" t="s">
         <v>524</v>
@@ -4630,7 +4631,7 @@
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B143" t="s">
         <v>524</v>
@@ -4638,7 +4639,7 @@
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B144" t="s">
         <v>524</v>
@@ -4646,7 +4647,7 @@
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B145" t="s">
         <v>524</v>
@@ -4654,7 +4655,7 @@
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B146" t="s">
         <v>524</v>
@@ -4662,7 +4663,7 @@
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B147" t="s">
         <v>524</v>
@@ -4670,7 +4671,7 @@
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B148" t="s">
         <v>524</v>
@@ -4678,7 +4679,7 @@
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B149" t="s">
         <v>524</v>
@@ -4686,7 +4687,7 @@
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B150" t="s">
         <v>524</v>
@@ -4694,7 +4695,7 @@
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B151" t="s">
         <v>524</v>
@@ -4702,7 +4703,7 @@
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B152" t="s">
         <v>524</v>
@@ -4710,7 +4711,7 @@
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B153" t="s">
         <v>524</v>
@@ -4718,7 +4719,7 @@
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B154" t="s">
         <v>524</v>
@@ -4726,7 +4727,7 @@
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B155" t="s">
         <v>524</v>
@@ -4734,7 +4735,7 @@
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B156" t="s">
         <v>524</v>
@@ -4742,7 +4743,7 @@
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B157" t="s">
         <v>524</v>
@@ -4750,7 +4751,7 @@
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B158" t="s">
         <v>524</v>
@@ -4758,7 +4759,7 @@
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B159" t="s">
         <v>524</v>
@@ -4766,7 +4767,7 @@
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B160" t="s">
         <v>524</v>
@@ -4774,7 +4775,7 @@
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B161" t="s">
         <v>524</v>
@@ -4782,7 +4783,7 @@
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B162" t="s">
         <v>524</v>
@@ -4790,7 +4791,7 @@
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B163" t="s">
         <v>524</v>
@@ -4798,7 +4799,7 @@
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B164" t="s">
         <v>524</v>
@@ -4806,7 +4807,7 @@
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B165" t="s">
         <v>524</v>
@@ -4814,7 +4815,7 @@
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B166" t="s">
         <v>524</v>
@@ -4822,7 +4823,7 @@
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B167" t="s">
         <v>524</v>
@@ -4830,7 +4831,7 @@
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B168" t="s">
         <v>524</v>
@@ -4838,7 +4839,7 @@
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B169" t="s">
         <v>524</v>
@@ -4846,7 +4847,7 @@
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B170" t="s">
         <v>524</v>
@@ -4854,7 +4855,7 @@
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B171" t="s">
         <v>524</v>
@@ -4862,7 +4863,7 @@
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B172" t="s">
         <v>524</v>
@@ -4870,7 +4871,7 @@
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B173" t="s">
         <v>524</v>
@@ -4878,7 +4879,7 @@
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B174" t="s">
         <v>524</v>
@@ -4886,7 +4887,7 @@
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B175" t="s">
         <v>524</v>
@@ -4894,7 +4895,7 @@
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B176" t="s">
         <v>524</v>
@@ -4902,7 +4903,7 @@
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B177" t="s">
         <v>524</v>
@@ -4910,7 +4911,7 @@
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B178" t="s">
         <v>524</v>
@@ -4918,7 +4919,7 @@
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B179" t="s">
         <v>524</v>
@@ -4926,7 +4927,7 @@
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B180" t="s">
         <v>524</v>
@@ -4934,7 +4935,7 @@
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B181" t="s">
         <v>524</v>
@@ -4942,7 +4943,7 @@
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B182" t="s">
         <v>524</v>
@@ -4950,7 +4951,7 @@
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B183" t="s">
         <v>524</v>
@@ -4958,7 +4959,7 @@
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B184" t="s">
         <v>524</v>
@@ -4966,7 +4967,7 @@
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B185" t="s">
         <v>524</v>
@@ -4974,15 +4975,15 @@
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>188</v>
+        <v>388</v>
       </c>
       <c r="B186" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>389</v>
+        <v>188</v>
       </c>
       <c r="B187" t="s">
         <v>525</v>
@@ -4990,7 +4991,7 @@
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>178</v>
+        <v>389</v>
       </c>
       <c r="B188" t="s">
         <v>525</v>
@@ -4998,7 +4999,7 @@
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B189" t="s">
         <v>525</v>
@@ -5006,7 +5007,7 @@
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>390</v>
+        <v>176</v>
       </c>
       <c r="B190" t="s">
         <v>525</v>
@@ -5014,7 +5015,7 @@
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>179</v>
+        <v>390</v>
       </c>
       <c r="B191" t="s">
         <v>525</v>
@@ -5022,7 +5023,7 @@
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>204</v>
+        <v>179</v>
       </c>
       <c r="B192" t="s">
         <v>525</v>
@@ -5030,7 +5031,7 @@
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>193</v>
+        <v>204</v>
       </c>
       <c r="B193" t="s">
         <v>525</v>
@@ -5038,7 +5039,7 @@
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>391</v>
+        <v>193</v>
       </c>
       <c r="B194" t="s">
         <v>525</v>
@@ -5046,7 +5047,7 @@
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>197</v>
+        <v>391</v>
       </c>
       <c r="B195" t="s">
         <v>525</v>
@@ -5054,7 +5055,7 @@
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>392</v>
+        <v>197</v>
       </c>
       <c r="B196" t="s">
         <v>525</v>
@@ -5062,7 +5063,7 @@
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B197" t="s">
         <v>525</v>
@@ -5070,7 +5071,7 @@
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>187</v>
+        <v>393</v>
       </c>
       <c r="B198" t="s">
         <v>525</v>
@@ -5078,7 +5079,7 @@
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>394</v>
+        <v>187</v>
       </c>
       <c r="B199" t="s">
         <v>525</v>
@@ -5086,7 +5087,7 @@
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>180</v>
+        <v>394</v>
       </c>
       <c r="B200" t="s">
         <v>525</v>
@@ -5094,7 +5095,7 @@
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B201" t="s">
         <v>525</v>
@@ -5102,7 +5103,7 @@
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B202" t="s">
         <v>525</v>
@@ -5110,7 +5111,7 @@
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="B203" t="s">
         <v>525</v>
@@ -5118,7 +5119,7 @@
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="B204" t="s">
         <v>525</v>
@@ -5126,7 +5127,7 @@
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
-        <v>395</v>
+        <v>194</v>
       </c>
       <c r="B205" t="s">
         <v>525</v>
@@ -5134,7 +5135,7 @@
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B206" t="s">
         <v>525</v>
@@ -5142,7 +5143,7 @@
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
-        <v>190</v>
+        <v>396</v>
       </c>
       <c r="B207" t="s">
         <v>525</v>
@@ -5150,7 +5151,7 @@
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
-        <v>397</v>
+        <v>190</v>
       </c>
       <c r="B208" t="s">
         <v>525</v>
@@ -5158,7 +5159,7 @@
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B209" t="s">
         <v>525</v>
@@ -5166,7 +5167,7 @@
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
-        <v>191</v>
+        <v>398</v>
       </c>
       <c r="B210" t="s">
         <v>525</v>
@@ -5174,7 +5175,7 @@
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
-        <v>399</v>
+        <v>191</v>
       </c>
       <c r="B211" t="s">
         <v>525</v>
@@ -5182,7 +5183,7 @@
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
-        <v>202</v>
+        <v>399</v>
       </c>
       <c r="B212" t="s">
         <v>525</v>
@@ -5190,7 +5191,7 @@
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B213" t="s">
         <v>525</v>
@@ -5198,7 +5199,7 @@
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
-        <v>400</v>
+        <v>205</v>
       </c>
       <c r="B214" t="s">
         <v>525</v>
@@ -5206,7 +5207,7 @@
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
-        <v>203</v>
+        <v>400</v>
       </c>
       <c r="B215" t="s">
         <v>525</v>
@@ -5214,7 +5215,7 @@
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
-        <v>401</v>
+        <v>203</v>
       </c>
       <c r="B216" t="s">
         <v>525</v>
@@ -5222,7 +5223,7 @@
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
-        <v>201</v>
+        <v>401</v>
       </c>
       <c r="B217" t="s">
         <v>525</v>
@@ -5230,7 +5231,7 @@
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
-        <v>184</v>
+        <v>201</v>
       </c>
       <c r="B218" t="s">
         <v>525</v>
@@ -5238,7 +5239,7 @@
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
-        <v>402</v>
+        <v>184</v>
       </c>
       <c r="B219" t="s">
         <v>525</v>
@@ -5246,7 +5247,7 @@
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B220" t="s">
         <v>525</v>
@@ -5254,7 +5255,7 @@
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B221" t="s">
         <v>525</v>
@@ -5262,7 +5263,7 @@
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
-        <v>199</v>
+        <v>404</v>
       </c>
       <c r="B222" t="s">
         <v>525</v>
@@ -5270,7 +5271,7 @@
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
-        <v>192</v>
+        <v>199</v>
       </c>
       <c r="B223" t="s">
         <v>525</v>
@@ -5278,7 +5279,7 @@
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
-        <v>185</v>
+        <v>192</v>
       </c>
       <c r="B224" t="s">
         <v>525</v>
@@ -5286,7 +5287,7 @@
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
-        <v>198</v>
+        <v>185</v>
       </c>
       <c r="B225" t="s">
         <v>525</v>
@@ -5294,7 +5295,7 @@
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="B226" t="s">
         <v>525</v>
@@ -5302,7 +5303,7 @@
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B227" t="s">
         <v>525</v>
@@ -5310,7 +5311,7 @@
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
-        <v>186</v>
+        <v>196</v>
       </c>
       <c r="B228" t="s">
         <v>525</v>
@@ -5318,7 +5319,7 @@
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
-        <v>200</v>
+        <v>186</v>
       </c>
       <c r="B229" t="s">
         <v>525</v>
@@ -5326,15 +5327,15 @@
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
-        <v>405</v>
+        <v>200</v>
       </c>
       <c r="B230" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B231" t="s">
         <v>526</v>
@@ -5342,7 +5343,7 @@
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B232" t="s">
         <v>526</v>
@@ -5350,7 +5351,7 @@
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B233" t="s">
         <v>526</v>
@@ -5358,7 +5359,7 @@
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B234" t="s">
         <v>526</v>
@@ -5366,7 +5367,7 @@
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B235" t="s">
         <v>526</v>
@@ -5374,7 +5375,7 @@
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B236" t="s">
         <v>526</v>
@@ -5382,7 +5383,7 @@
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B237" t="s">
         <v>526</v>
@@ -5390,7 +5391,7 @@
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B238" t="s">
         <v>526</v>
@@ -5398,7 +5399,7 @@
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B239" t="s">
         <v>526</v>
@@ -5406,7 +5407,7 @@
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B240" t="s">
         <v>526</v>
@@ -5414,7 +5415,7 @@
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B241" t="s">
         <v>526</v>
@@ -5422,7 +5423,7 @@
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B242" t="s">
         <v>526</v>
@@ -5430,7 +5431,7 @@
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B243" t="s">
         <v>526</v>
@@ -5438,7 +5439,7 @@
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B244" t="s">
         <v>526</v>
@@ -5446,7 +5447,7 @@
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B245" t="s">
         <v>526</v>
@@ -5454,7 +5455,7 @@
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B246" t="s">
         <v>526</v>
@@ -5462,7 +5463,7 @@
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B247" t="s">
         <v>526</v>
@@ -5470,7 +5471,7 @@
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B248" t="s">
         <v>526</v>
@@ -5478,7 +5479,7 @@
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B249" t="s">
         <v>526</v>
@@ -5486,7 +5487,7 @@
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B250" t="s">
         <v>526</v>
@@ -5494,7 +5495,7 @@
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B251" t="s">
         <v>526</v>
@@ -5502,7 +5503,7 @@
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B252" t="s">
         <v>526</v>
@@ -5510,7 +5511,7 @@
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B253" t="s">
         <v>526</v>
@@ -5518,7 +5519,7 @@
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B254" t="s">
         <v>526</v>
@@ -5526,15 +5527,15 @@
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B255" t="s">
-        <v>448</v>
+        <v>526</v>
       </c>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B256" t="s">
         <v>448</v>
@@ -5542,7 +5543,7 @@
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B257" t="s">
         <v>448</v>
@@ -5550,7 +5551,7 @@
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B258" t="s">
         <v>448</v>
@@ -5558,7 +5559,7 @@
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B259" t="s">
         <v>448</v>
@@ -5566,7 +5567,7 @@
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B260" t="s">
         <v>448</v>
@@ -5574,7 +5575,7 @@
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B261" t="s">
         <v>448</v>
@@ -5582,7 +5583,7 @@
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B262" t="s">
         <v>448</v>
@@ -5590,7 +5591,7 @@
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B263" t="s">
         <v>448</v>
@@ -5598,7 +5599,7 @@
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A264" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B264" t="s">
         <v>448</v>
@@ -5606,7 +5607,7 @@
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B265" t="s">
         <v>448</v>
@@ -5614,7 +5615,7 @@
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A266" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B266" t="s">
         <v>448</v>
@@ -5622,7 +5623,7 @@
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A267" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B267" t="s">
         <v>448</v>
@@ -5630,7 +5631,7 @@
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A268" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B268" t="s">
         <v>448</v>
@@ -5638,7 +5639,7 @@
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A269" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B269" t="s">
         <v>448</v>
@@ -5646,7 +5647,7 @@
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A270" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B270" t="s">
         <v>448</v>
@@ -5654,7 +5655,7 @@
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A271" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B271" t="s">
         <v>448</v>
@@ -5662,7 +5663,7 @@
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A272" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B272" t="s">
         <v>448</v>
@@ -5670,7 +5671,7 @@
     </row>
     <row r="273" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A273" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B273" t="s">
         <v>448</v>
@@ -5678,7 +5679,7 @@
     </row>
     <row r="274" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A274" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B274" t="s">
         <v>448</v>
@@ -5686,7 +5687,7 @@
     </row>
     <row r="275" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A275" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B275" t="s">
         <v>448</v>
@@ -5694,7 +5695,7 @@
     </row>
     <row r="276" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A276" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B276" t="s">
         <v>448</v>
@@ -5702,7 +5703,7 @@
     </row>
     <row r="277" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A277" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B277" t="s">
         <v>448</v>
@@ -5710,7 +5711,7 @@
     </row>
     <row r="278" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A278" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B278" t="s">
         <v>448</v>
@@ -5718,7 +5719,7 @@
     </row>
     <row r="279" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A279" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B279" t="s">
         <v>448</v>
@@ -5726,7 +5727,7 @@
     </row>
     <row r="280" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A280" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B280" t="s">
         <v>448</v>
@@ -5734,15 +5735,15 @@
     </row>
     <row r="281" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A281" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B281" t="s">
-        <v>527</v>
+        <v>448</v>
       </c>
     </row>
     <row r="282" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A282" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B282" t="s">
         <v>527</v>
@@ -5750,7 +5751,7 @@
     </row>
     <row r="283" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A283" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B283" t="s">
         <v>527</v>
@@ -5758,7 +5759,7 @@
     </row>
     <row r="284" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A284" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B284" t="s">
         <v>527</v>
@@ -5766,7 +5767,7 @@
     </row>
     <row r="285" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A285" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B285" t="s">
         <v>527</v>
@@ -5774,7 +5775,7 @@
     </row>
     <row r="286" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A286" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B286" t="s">
         <v>527</v>
@@ -5782,7 +5783,7 @@
     </row>
     <row r="287" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A287" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B287" t="s">
         <v>527</v>
@@ -5790,7 +5791,7 @@
     </row>
     <row r="288" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A288" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B288" t="s">
         <v>527</v>
@@ -5798,7 +5799,7 @@
     </row>
     <row r="289" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A289" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B289" t="s">
         <v>527</v>
@@ -5806,7 +5807,7 @@
     </row>
     <row r="290" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A290" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B290" t="s">
         <v>527</v>
@@ -5814,7 +5815,7 @@
     </row>
     <row r="291" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A291" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B291" t="s">
         <v>527</v>
@@ -5822,7 +5823,7 @@
     </row>
     <row r="292" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A292" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B292" t="s">
         <v>527</v>
@@ -5830,7 +5831,7 @@
     </row>
     <row r="293" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A293" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B293" t="s">
         <v>527</v>
@@ -5838,15 +5839,15 @@
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A294" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B294" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="295" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A295" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B295" t="s">
         <v>528</v>
@@ -5854,7 +5855,7 @@
     </row>
     <row r="296" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A296" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B296" t="s">
         <v>528</v>
@@ -5862,7 +5863,7 @@
     </row>
     <row r="297" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A297" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B297" t="s">
         <v>528</v>
@@ -5870,7 +5871,7 @@
     </row>
     <row r="298" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A298" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B298" t="s">
         <v>528</v>
@@ -5878,7 +5879,7 @@
     </row>
     <row r="299" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A299" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B299" t="s">
         <v>528</v>
@@ -5886,7 +5887,7 @@
     </row>
     <row r="300" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A300" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B300" t="s">
         <v>528</v>
@@ -5894,7 +5895,7 @@
     </row>
     <row r="301" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A301" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B301" t="s">
         <v>528</v>
@@ -5902,7 +5903,7 @@
     </row>
     <row r="302" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A302" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B302" t="s">
         <v>528</v>
@@ -5910,7 +5911,7 @@
     </row>
     <row r="303" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A303" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B303" t="s">
         <v>528</v>
@@ -5918,7 +5919,7 @@
     </row>
     <row r="304" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A304" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B304" t="s">
         <v>528</v>
@@ -5926,7 +5927,7 @@
     </row>
     <row r="305" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A305" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B305" t="s">
         <v>528</v>
@@ -5934,7 +5935,7 @@
     </row>
     <row r="306" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A306" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B306" t="s">
         <v>528</v>
@@ -5942,7 +5943,7 @@
     </row>
     <row r="307" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A307" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B307" t="s">
         <v>528</v>
@@ -5950,7 +5951,7 @@
     </row>
     <row r="308" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A308" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B308" t="s">
         <v>528</v>
@@ -5958,7 +5959,7 @@
     </row>
     <row r="309" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A309" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B309" t="s">
         <v>528</v>
@@ -5966,7 +5967,7 @@
     </row>
     <row r="310" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A310" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="B310" t="s">
         <v>528</v>
@@ -5974,7 +5975,7 @@
     </row>
     <row r="311" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A311" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B311" t="s">
         <v>528</v>
@@ -5982,7 +5983,7 @@
     </row>
     <row r="312" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A312" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B312" t="s">
         <v>528</v>
@@ -5990,7 +5991,7 @@
     </row>
     <row r="313" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A313" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B313" t="s">
         <v>528</v>
@@ -5998,7 +5999,7 @@
     </row>
     <row r="314" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A314" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B314" t="s">
         <v>528</v>
@@ -6006,7 +6007,7 @@
     </row>
     <row r="315" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A315" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B315" t="s">
         <v>528</v>
@@ -6014,7 +6015,7 @@
     </row>
     <row r="316" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A316" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B316" t="s">
         <v>528</v>
@@ -6022,7 +6023,7 @@
     </row>
     <row r="317" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A317" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B317" t="s">
         <v>528</v>
@@ -6030,7 +6031,7 @@
     </row>
     <row r="318" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A318" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="B318" t="s">
         <v>528</v>
@@ -6038,7 +6039,7 @@
     </row>
     <row r="319" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A319" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B319" t="s">
         <v>528</v>
@@ -6046,7 +6047,7 @@
     </row>
     <row r="320" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A320" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B320" t="s">
         <v>528</v>
@@ -6054,7 +6055,7 @@
     </row>
     <row r="321" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A321" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B321" t="s">
         <v>528</v>
@@ -6062,7 +6063,7 @@
     </row>
     <row r="322" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A322" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B322" t="s">
         <v>528</v>
@@ -6070,7 +6071,7 @@
     </row>
     <row r="323" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A323" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B323" t="s">
         <v>528</v>
@@ -6078,7 +6079,7 @@
     </row>
     <row r="324" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A324" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="B324" t="s">
         <v>528</v>
@@ -6086,7 +6087,7 @@
     </row>
     <row r="325" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A325" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="B325" t="s">
         <v>528</v>
@@ -6094,7 +6095,7 @@
     </row>
     <row r="326" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A326" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="B326" t="s">
         <v>528</v>
@@ -6102,7 +6103,7 @@
     </row>
     <row r="327" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A327" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="B327" t="s">
         <v>528</v>
@@ -6110,7 +6111,7 @@
     </row>
     <row r="328" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A328" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="B328" t="s">
         <v>528</v>
@@ -6118,7 +6119,7 @@
     </row>
     <row r="329" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A329" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="B329" t="s">
         <v>528</v>
@@ -6126,7 +6127,7 @@
     </row>
     <row r="330" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A330" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="B330" t="s">
         <v>528</v>
@@ -6134,7 +6135,7 @@
     </row>
     <row r="331" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A331" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="B331" t="s">
         <v>528</v>
@@ -6142,7 +6143,7 @@
     </row>
     <row r="332" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A332" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="B332" t="s">
         <v>528</v>
@@ -6150,7 +6151,7 @@
     </row>
     <row r="333" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A333" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="B333" t="s">
         <v>528</v>
@@ -6158,7 +6159,7 @@
     </row>
     <row r="334" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A334" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B334" t="s">
         <v>528</v>
@@ -6166,7 +6167,7 @@
     </row>
     <row r="335" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A335" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B335" t="s">
         <v>528</v>
@@ -6174,7 +6175,7 @@
     </row>
     <row r="336" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A336" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="B336" t="s">
         <v>528</v>
@@ -6182,7 +6183,7 @@
     </row>
     <row r="337" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A337" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B337" t="s">
         <v>528</v>
@@ -6190,7 +6191,7 @@
     </row>
     <row r="338" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A338" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="B338" t="s">
         <v>528</v>
@@ -6198,7 +6199,7 @@
     </row>
     <row r="339" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A339" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="B339" t="s">
         <v>528</v>
@@ -6206,7 +6207,7 @@
     </row>
     <row r="340" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A340" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B340" t="s">
         <v>528</v>
@@ -6214,7 +6215,7 @@
     </row>
     <row r="341" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A341" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B341" t="s">
         <v>528</v>
@@ -6222,7 +6223,7 @@
     </row>
     <row r="342" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A342" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B342" t="s">
         <v>528</v>
@@ -6230,9 +6231,17 @@
     </row>
     <row r="343" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A343" t="s">
+        <v>517</v>
+      </c>
+      <c r="B343" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="344" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A344" t="s">
         <v>518</v>
       </c>
-      <c r="B343" t="s">
+      <c r="B344" t="s">
         <v>528</v>
       </c>
     </row>

</xml_diff>